<commit_message>
Finish the UpWork job
</commit_message>
<xml_diff>
--- a/implementation3/final.xlsx
+++ b/implementation3/final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alperen\Desktop\Alperen\github\My_Repositories\Learning_BeautifulSoup\implementation3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B76B931-11AE-4296-BABA-4F9B2A2C8D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{38810EBA-28C6-4650-8DDA-E20060134F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3509,7 +3509,7 @@
   <dimension ref="A1:E278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>